<commit_message>
#Fix Import Schüler xlsx
</commit_message>
<xml_diff>
--- a/Common/Style/Resource/Template/Import_Schueler.xlsx
+++ b/Common/Style/Resource/Template/Import_Schueler.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmiezik\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rackel\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFB1114-BD51-4BCE-B57F-9E98BAD67975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E60077-092C-4086-A77A-1C8782153731}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schüler" sheetId="1" r:id="rId1"/>
@@ -639,9 +639,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -679,7 +679,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -785,7 +785,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -927,7 +927,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -941,7 +941,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1612,12 +1612,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="KcSU4hspeK+/6PhDslRzTV/jc+cYEZvWRpgPEgUK80yFN5YM2DoCz/rTKtZCkeLU43RKQSzUZdnywKsXOuuYRw==" saltValue="1bVHAM0UJKYMIe3iECspPQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" autoFilter="0"/>
-  <autoFilter ref="A2:CP2" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:CP376">
-      <sortCondition ref="A1:A376"/>
-    </sortState>
-  </autoFilter>
+  <sheetProtection algorithmName="SHA-512" hashValue="zQtwzR231FgHfViik8z3XA1Cnsy5ILke1R4ga2evVoPHg+SgnT1j2G3W/n8bVwfI4TdiJdBsn7b3TVO9tJdw8w==" saltValue="vfG4llJKMyM6oMVfXrShzg==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" autoFilter="0"/>
+  <autoFilter ref="A2:CP2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>